<commit_message>
slm restructuring json blob for contentful api
</commit_message>
<xml_diff>
--- a/site-page/scrape_sample.xlsx
+++ b/site-page/scrape_sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21320"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amaynard\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F774467B-730E-410D-B4B2-0B9379294B79}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5014E2AE-021E-4539-8ADC-66371D0A47FC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19160" windowHeight="6920" xr2:uid="{D1438603-BFC8-44B3-BD21-A42FE6748477}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="37">
   <si>
     <t>URL</t>
   </si>
@@ -48,19 +48,8 @@
     <t>Includes Text Shared with Other Products</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Audience
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>(student, teacher, school administrator, district administrator, parent, counselor, implementation coordinator)</t>
-    </r>
+    <t>Audience
+(student, teacher, site administrator, district administrator, parent, counselor, implementation coordinator)</t>
   </si>
   <si>
     <t>Scrape? 
@@ -82,37 +71,43 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Teacher, School Administrator, District Administrator, Counselor, Implementation Coordinator</t>
-  </si>
-  <si>
-    <t>http://www.secondstep.org/Kindergarten/Program-Coordinators/Second-Step-Kit/Evaluation-Guide/Evaluation-Design</t>
+    <t>Teacher, Site Administrator, District Administrator, Counselor, Implementation Coordinator</t>
+  </si>
+  <si>
+    <t>http://www.secondstep.org/Kindergarten/Program-Coordinators/Second-Step-Kit/evaluation-guide/Evaluating-Implementation</t>
+  </si>
+  <si>
+    <t>Evaluating Implementation</t>
+  </si>
+  <si>
+    <t>http://www.secondstep.org/Kindergarten/Program-Coordinators/Second-Step-Kit/evaluation-guide/evaluation-design</t>
   </si>
   <si>
     <t>Evaluation Design</t>
   </si>
   <si>
-    <t>http://www.secondstep.org/Kindergarten/Program-Coordinators/Second-Step-Kit/Evaluation-Guide/Outcome-Measures</t>
+    <t>http://www.secondstep.org/Kindergarten/Program-Coordinators/Second-Step-Kit/evaluation-guide/using-school-data</t>
+  </si>
+  <si>
+    <t>Using School Data</t>
+  </si>
+  <si>
+    <t>http://www.secondstep.org/Kindergarten/Program-Coordinators/Second-Step-Kit/Evaluation-Guidehttp://www.secondstep.org/Kindergarten/Program-Coordinators/Second-Step-Kit/evaluation-guide/using-evaluation-results</t>
+  </si>
+  <si>
+    <t>Using Evaluation Results</t>
+  </si>
+  <si>
+    <t>http://www.secondstep.org/Kindergarten/Program-Coordinators/Second-Step-Kit/Evaluation-Guidehttp://www.secondstep.org/Kindergarten/Program-Coordinators/Second-Step-Kit/evaluation-guide/Outcome-Measures</t>
   </si>
   <si>
     <t>Outcome Measures</t>
   </si>
   <si>
-    <t>http://www.secondstep.org/Kindergarten/Program-Coordinators/Second-Step-Kit/Evaluation-Guide/Using-Data</t>
-  </si>
-  <si>
-    <t>Using Data for Evaluation</t>
-  </si>
-  <si>
-    <t>http://www.secondstep.org/Kindergarten/Program-Coordinators/Second-Step-Kit/Evaluation-Guide/Using-Evaluation-Findings</t>
-  </si>
-  <si>
-    <t>Using Evaluation Findings</t>
-  </si>
-  <si>
-    <t>http://www.secondstep.org/Kindergarten/Program-Coordinators/Second-Step-Kit/Evaluation-Guide/Evaluating-Implementation</t>
-  </si>
-  <si>
-    <t>Evaluating Implementation</t>
+    <t>http://www.secondstep.org/Kindergarten/Program-Coordinators/Second-Step-Kit/Evaluation-Guidehttp://www.secondstep.org/Kindergarten/Program-Coordinators/Second-Step-Kit/evaluation-guide/More-Evaluation-Tools</t>
+  </si>
+  <si>
+    <t>More Evaluation Tools</t>
   </si>
   <si>
     <t>File Name</t>
@@ -149,12 +144,6 @@
   </si>
   <si>
     <t>n/a</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>teacher, school administrator, district administrator, counselor, implementation coordinator</t>
   </si>
 </sst>
 </file>
@@ -326,7 +315,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -349,12 +338,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -377,6 +360,13 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -692,10 +682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA1EF95E-E720-4E49-B0BA-585448560E9B}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0" xr3:uid="{51963EF1-B21D-5CDC-8E1D-FB35BE00368E}">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0" xr3:uid="{51963EF1-B21D-5CDC-8E1D-FB35BE00368E}">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -703,7 +693,7 @@
     <col min="1" max="8" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="81.95" thickBot="1">
+    <row r="1" spans="1:7" ht="120.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -722,11 +712,11 @@
       <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="87.95" thickTop="1">
+    <row r="2" spans="1:7" ht="86.25">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -745,11 +735,11 @@
       <c r="F2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="87.6">
+    <row r="3" spans="1:7" ht="86.25">
       <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
@@ -768,12 +758,12 @@
       <c r="F3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="87.6">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:7" ht="86.25">
+      <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -791,11 +781,11 @@
       <c r="F4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="87.6">
+    <row r="5" spans="1:7" ht="86.25">
       <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
@@ -814,15 +804,15 @@
       <c r="F5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="87.6">
+    <row r="6" spans="1:7" ht="120">
       <c r="A6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -837,15 +827,15 @@
       <c r="F6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="87.6">
+    <row r="7" spans="1:7" ht="120">
       <c r="A7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="6" t="s">
@@ -860,18 +850,42 @@
       <c r="F7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="120">
+      <c r="A8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="15" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="http://www.secondstep.org/Early-Learning/Program-Coordinators/Second-Step-Kit/Evaluation-Guide" xr:uid="{0BF1EF89-9F23-41EB-B984-F8D89ED94123}"/>
-    <hyperlink ref="A3" r:id="rId2" display="http://www.secondstep.org/Early-Learning/Program-Coordinators/Second-Step-Kit/Evaluation-Guide/Evaluation-Design" xr:uid="{DB8C259F-4263-4E39-93B5-31F5A82C32E0}"/>
-    <hyperlink ref="A4" r:id="rId3" display="http://www.secondstep.org/Early-Learning/Program-Coordinators/Second-Step-Kit/Evaluation-Guide/Outcome-Measures" xr:uid="{9877AF36-45D1-45D6-A820-9C1E6172D6DA}"/>
-    <hyperlink ref="A5" r:id="rId4" display="http://www.secondstep.org/Early-Learning/Program-Coordinators/Second-Step-Kit/Evaluation-Guide/Using-Data" xr:uid="{2D4D529C-DC6E-44AF-9016-717CD8BA4082}"/>
-    <hyperlink ref="A6" r:id="rId5" display="http://www.secondstep.org/Early-Learning/Program-Coordinators/Second-Step-Kit/Evaluation-Guide/Using-Evaluation-Findings" xr:uid="{94808C63-BB2B-495E-A038-B0192771260C}"/>
-    <hyperlink ref="A7" r:id="rId6" display="http://www.secondstep.org/Early-Learning/Program-Coordinators/Second-Step-Kit/Evaluation-Guide/Evaluating-Implementation" xr:uid="{AAE6C55E-B550-400A-8FAD-E6652C7BDC2C}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{30C6683B-A065-4E31-94D3-67912FC876B7}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{47D8218A-5069-40F9-BCCB-CB40E0F4C309}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{4CA81ECC-2C61-4342-9F85-CED1B4A58635}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{303F510D-35A6-4FD1-B9E9-8D7417CB0B9D}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{0BBAA87B-78DB-46F8-B617-9CC966FDB49E}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{A914D74B-E990-4282-94D7-4B186E5F5FFB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -882,7 +896,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0" xr3:uid="{586C0002-B8A0-53EB-86BF-267805AEB518}">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -890,78 +904,78 @@
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="8" max="8" width="10" style="18" customWidth="1"/>
     <col min="9" max="9" width="27.42578125" customWidth="1"/>
     <col min="11" max="11" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="13" customFormat="1" ht="80.45" thickBot="1">
-      <c r="A1" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="11" t="s">
+    <row r="1" spans="1:11" s="11" customFormat="1" ht="85.5">
+      <c r="A1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="B1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="11" t="s">
+      <c r="E1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" s="10" t="s">
+      <c r="H1" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>30</v>
+      <c r="J1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="15" customFormat="1" ht="53.1" thickTop="1">
-      <c r="A2" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="14" t="s">
+    <row r="2" spans="1:11" s="13" customFormat="1" ht="69">
+      <c r="A2" s="12" t="s">
         <v>33</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>35</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>34</v>
+      <c r="E2" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>36</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="14"/>
+      <c r="H2" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" s="12"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -975,8 +989,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007245679789E3B040A6E9B3D2CEA4C25D" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4486521d365a727f4ba283df0563b06d">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="30c32527-9772-45f6-81fd-eb119666bd10" xmlns:ns3="2736ec62-27d7-4568-92c6-5505e2b7bb1a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="74907c4524589df772a2551802221f35" ns2:_="" ns3:_="">
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007245679789E3B040A6E9B3D2CEA4C25D" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b177a10fb654477513820576e7b0f396">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="30c32527-9772-45f6-81fd-eb119666bd10" xmlns:ns3="2736ec62-27d7-4568-92c6-5505e2b7bb1a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9f29b06bdcd29c7588d1ca5dc418c4a2" ns2:_="" ns3:_="">
     <xsd:import namespace="30c32527-9772-45f6-81fd-eb119666bd10"/>
     <xsd:import namespace="2736ec62-27d7-4568-92c6-5505e2b7bb1a"/>
     <xsd:element name="properties">
@@ -989,6 +1012,9 @@
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1007,6 +1033,23 @@
     <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="14" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -1139,29 +1182,20 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0CBEB87-F7C3-4DE3-87B9-83D8B61C36BC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D60547B-B828-4FD5-8F29-707D3A36D7E7}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28EB1826-AB13-4AD2-A90C-9C5F4E82C7E0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB49EC49-274C-48BE-A620-BAA0C5C81AB0}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D60547B-B828-4FD5-8F29-707D3A36D7E7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28EB1826-AB13-4AD2-A90C-9C5F4E82C7E0}"/>
 </file>
</xml_diff>